<commit_message>
Atualização do Relatório Mensal de Pagamentos das OS - Ref. 2ª Quinzena de Nov/2016.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201611-2.xlsx
+++ b/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201611-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Acumulado" sheetId="13" r:id="rId1"/>
@@ -1719,11 +1719,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3567,11 +3567,11 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4424,11 +4424,11 @@
   </sheetPr>
   <dimension ref="A1:AG154"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="I65" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F66" sqref="F66:N66"/>
+      <selection pane="bottomRight" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,12 +4500,12 @@
       <c r="A3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
       <c r="F3" s="26" t="s">
         <v>108</v>
       </c>
@@ -4613,11 +4613,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4721</v>
       </c>
-      <c r="B5" s="115" t="str">
+      <c r="B5" s="114" t="str">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C5" s="115"/>
+      <c r="C5" s="114"/>
       <c r="D5" s="52" t="str">
         <f>IF(A5="","","em")</f>
         <v>em</v>
@@ -5036,11 +5036,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4757</v>
       </c>
-      <c r="B10" s="115" t="str">
+      <c r="B10" s="114" t="str">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C10" s="115"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="52" t="str">
         <f>IF(A10="","","em")</f>
         <v>em</v>
@@ -5459,11 +5459,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4776</v>
       </c>
-      <c r="B15" s="115" t="str">
+      <c r="B15" s="114" t="str">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Devolvida</v>
       </c>
-      <c r="C15" s="115"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="52" t="str">
         <f>IF(A15="","","em")</f>
         <v>em</v>
@@ -5882,11 +5882,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4777</v>
       </c>
-      <c r="B20" s="115" t="str">
+      <c r="B20" s="114" t="str">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Devolvida</v>
       </c>
-      <c r="C20" s="115"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="52" t="str">
         <f>IF(A20="","","em")</f>
         <v>em</v>
@@ -6305,11 +6305,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4782</v>
       </c>
-      <c r="B25" s="115" t="str">
+      <c r="B25" s="114" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Devolvida</v>
       </c>
-      <c r="C25" s="115"/>
+      <c r="C25" s="114"/>
       <c r="D25" s="52" t="str">
         <f>IF(A25="","","em")</f>
         <v>em</v>
@@ -6728,11 +6728,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4797</v>
       </c>
-      <c r="B30" s="115" t="str">
+      <c r="B30" s="114" t="str">
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Entregue</v>
       </c>
-      <c r="C30" s="115"/>
+      <c r="C30" s="114"/>
       <c r="D30" s="52" t="str">
         <f>IF(A30="","","em")</f>
         <v>em</v>
@@ -7151,11 +7151,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4808</v>
       </c>
-      <c r="B35" s="115" t="str">
+      <c r="B35" s="114" t="str">
         <f>IF(A35="","",VLOOKUP(A35,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C35" s="115"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="52" t="str">
         <f>IF(A35="","","em")</f>
         <v>em</v>
@@ -7574,11 +7574,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4809</v>
       </c>
-      <c r="B40" s="115" t="str">
+      <c r="B40" s="114" t="str">
         <f>IF(A40="","",VLOOKUP(A40,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C40" s="115"/>
+      <c r="C40" s="114"/>
       <c r="D40" s="52" t="str">
         <f>IF(A40="","","em")</f>
         <v>em</v>
@@ -7997,11 +7997,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4810</v>
       </c>
-      <c r="B45" s="115" t="str">
+      <c r="B45" s="114" t="str">
         <f>IF(A45="","",VLOOKUP(A45,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Paralisada</v>
       </c>
-      <c r="C45" s="115"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="52" t="str">
         <f>IF(A45="","","em")</f>
         <v>em</v>
@@ -8420,11 +8420,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4813</v>
       </c>
-      <c r="B50" s="115" t="str">
+      <c r="B50" s="114" t="str">
         <f>IF(A50="","",VLOOKUP(A50,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Reiniciada</v>
       </c>
-      <c r="C50" s="115"/>
+      <c r="C50" s="114"/>
       <c r="D50" s="52" t="str">
         <f>IF(A50="","","em")</f>
         <v>em</v>
@@ -8843,11 +8843,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4817</v>
       </c>
-      <c r="B55" s="115" t="str">
+      <c r="B55" s="114" t="str">
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Aberta</v>
       </c>
-      <c r="C55" s="115"/>
+      <c r="C55" s="114"/>
       <c r="D55" s="52" t="str">
         <f>IF(A55="","","em")</f>
         <v>em</v>
@@ -9266,11 +9266,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4818</v>
       </c>
-      <c r="B60" s="115" t="str">
+      <c r="B60" s="114" t="str">
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Aberta</v>
       </c>
-      <c r="C60" s="115"/>
+      <c r="C60" s="114"/>
       <c r="D60" s="52" t="str">
         <f>IF(A60="","","em")</f>
         <v>em</v>
@@ -9689,11 +9689,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v>4819</v>
       </c>
-      <c r="B65" s="115" t="str">
+      <c r="B65" s="114" t="str">
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v>Aberta</v>
       </c>
-      <c r="C65" s="115"/>
+      <c r="C65" s="114"/>
       <c r="D65" s="52" t="str">
         <f>IF(A65="","","em")</f>
         <v>em</v>
@@ -10112,11 +10112,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B70" s="115" t="str">
+      <c r="B70" s="114" t="str">
         <f>IF(A70="","",VLOOKUP(A70,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C70" s="115"/>
+      <c r="C70" s="114"/>
       <c r="D70" s="52" t="str">
         <f>IF(A70="","","em")</f>
         <v/>
@@ -10535,11 +10535,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B75" s="115" t="str">
+      <c r="B75" s="114" t="str">
         <f>IF(A75="","",VLOOKUP(A75,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C75" s="115"/>
+      <c r="C75" s="114"/>
       <c r="D75" s="52" t="str">
         <f>IF(A75="","","em")</f>
         <v/>
@@ -10958,11 +10958,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B80" s="115" t="str">
+      <c r="B80" s="114" t="str">
         <f>IF(A80="","",VLOOKUP(A80,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C80" s="115"/>
+      <c r="C80" s="114"/>
       <c r="D80" s="52" t="str">
         <f>IF(A80="","","em")</f>
         <v/>
@@ -11381,11 +11381,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B85" s="115" t="str">
+      <c r="B85" s="114" t="str">
         <f>IF(A85="","",VLOOKUP(A85,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C85" s="115"/>
+      <c r="C85" s="114"/>
       <c r="D85" s="52" t="str">
         <f>IF(A85="","","em")</f>
         <v/>
@@ -11804,11 +11804,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B90" s="115" t="str">
+      <c r="B90" s="114" t="str">
         <f>IF(A90="","",VLOOKUP(A90,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C90" s="115"/>
+      <c r="C90" s="114"/>
       <c r="D90" s="52" t="str">
         <f>IF(A90="","","em")</f>
         <v/>
@@ -12227,11 +12227,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B95" s="115" t="str">
+      <c r="B95" s="114" t="str">
         <f>IF(A95="","",VLOOKUP(A95,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C95" s="115"/>
+      <c r="C95" s="114"/>
       <c r="D95" s="52" t="str">
         <f>IF(A95="","","em")</f>
         <v/>
@@ -12650,11 +12650,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B100" s="115" t="str">
+      <c r="B100" s="114" t="str">
         <f>IF(A100="","",VLOOKUP(A100,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C100" s="115"/>
+      <c r="C100" s="114"/>
       <c r="D100" s="52" t="str">
         <f>IF(A100="","","em")</f>
         <v/>
@@ -13073,11 +13073,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B105" s="115" t="str">
+      <c r="B105" s="114" t="str">
         <f>IF(A105="","",VLOOKUP(A105,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C105" s="115"/>
+      <c r="C105" s="114"/>
       <c r="D105" s="52" t="str">
         <f>IF(A105="","","em")</f>
         <v/>
@@ -13496,11 +13496,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B110" s="115" t="str">
+      <c r="B110" s="114" t="str">
         <f>IF(A110="","",VLOOKUP(A110,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C110" s="115"/>
+      <c r="C110" s="114"/>
       <c r="D110" s="52" t="str">
         <f>IF(A110="","","em")</f>
         <v/>
@@ -13919,11 +13919,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B115" s="115" t="str">
+      <c r="B115" s="114" t="str">
         <f>IF(A115="","",VLOOKUP(A115,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C115" s="115"/>
+      <c r="C115" s="114"/>
       <c r="D115" s="52" t="str">
         <f>IF(A115="","","em")</f>
         <v/>
@@ -14342,11 +14342,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B120" s="115" t="str">
+      <c r="B120" s="114" t="str">
         <f>IF(A120="","",VLOOKUP(A120,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C120" s="115"/>
+      <c r="C120" s="114"/>
       <c r="D120" s="52" t="str">
         <f>IF(A120="","","em")</f>
         <v/>
@@ -14765,11 +14765,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B125" s="115" t="str">
+      <c r="B125" s="114" t="str">
         <f>IF(A125="","",VLOOKUP(A125,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C125" s="115"/>
+      <c r="C125" s="114"/>
       <c r="D125" s="52" t="str">
         <f>IF(A125="","","em")</f>
         <v/>
@@ -15188,11 +15188,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B130" s="115" t="str">
+      <c r="B130" s="114" t="str">
         <f>IF(A130="","",VLOOKUP(A130,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C130" s="115"/>
+      <c r="C130" s="114"/>
       <c r="D130" s="52" t="str">
         <f>IF(A130="","","em")</f>
         <v/>
@@ -15611,11 +15611,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B135" s="115" t="str">
+      <c r="B135" s="114" t="str">
         <f>IF(A135="","",VLOOKUP(A135,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C135" s="115"/>
+      <c r="C135" s="114"/>
       <c r="D135" s="52" t="str">
         <f>IF(A135="","","em")</f>
         <v/>
@@ -16034,11 +16034,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B140" s="115" t="str">
+      <c r="B140" s="114" t="str">
         <f>IF(A140="","",VLOOKUP(A140,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C140" s="115"/>
+      <c r="C140" s="114"/>
       <c r="D140" s="52" t="str">
         <f>IF(A140="","","em")</f>
         <v/>
@@ -16457,11 +16457,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B145" s="115" t="str">
+      <c r="B145" s="114" t="str">
         <f>IF(A145="","",VLOOKUP(A145,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C145" s="115"/>
+      <c r="C145" s="114"/>
       <c r="D145" s="52" t="str">
         <f>IF(A145="","","em")</f>
         <v/>
@@ -16880,11 +16880,11 @@
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSCTL[],2,FALSE),""))</f>
         <v/>
       </c>
-      <c r="B150" s="115" t="str">
+      <c r="B150" s="114" t="str">
         <f>IF(A150="","",VLOOKUP(A150,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="C150" s="115"/>
+      <c r="C150" s="114"/>
       <c r="D150" s="52" t="str">
         <f>IF(A150="","","em")</f>
         <v/>
@@ -17300,37 +17300,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B120:C120"/>
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B135:C135"/>
     <mergeCell ref="B140:C140"/>
     <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">

</xml_diff>

<commit_message>
Atualização do Boletim de Acompanhamento, Relatório Mensal de Pagamentos das OS e Oficio de Autorização de Faturamento Mensal, referente a 1ª Quinzena de Nov/2016, e revisão dos documentos de acompanhamento das OS 4776, 4777, 4782, 4809, 4817, 4818 e 4819.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201611-2.xlsx
+++ b/00_GESTAO_GERAL/00_COMITE/04_RELATORIO_MENSAL/Relatóro Mensal de Ordens de Serviços - 201611-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Acumulado" sheetId="13" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="214">
   <si>
     <t>Número OS</t>
   </si>
@@ -844,7 +844,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,12 +884,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1424,7 +1418,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1719,9 +1713,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1779,7 +1771,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -2939,8 +2930,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2949,7 @@
       </c>
       <c r="D1" s="86">
         <f>D2*$G$1</f>
-        <v>865620</v>
+        <v>798210</v>
       </c>
       <c r="E1" s="86">
         <f>E2*$G$1</f>
@@ -2978,7 +2969,7 @@
       </c>
       <c r="D2" s="106">
         <f>SUM(Acumulado[PF Contratado])</f>
-        <v>1374</v>
+        <v>1267</v>
       </c>
       <c r="E2" s="108">
         <f>SUM(Acumulado[PF Faturado])</f>
@@ -2986,7 +2977,7 @@
       </c>
       <c r="F2" s="107">
         <f>C2-D2</f>
-        <v>2053</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -3018,7 +3009,7 @@
       </c>
       <c r="D4" s="21">
         <f>SUMIF(OSS[Código Processo],Acumulado[[#This Row],[Código Processo]],OSS[PF Previsto])</f>
-        <v>278</v>
+        <v>171</v>
       </c>
       <c r="E4" s="21">
         <f>SUMIF(OSS[Código Processo],Acumulado[[#This Row],[Código Processo]],OSS[PF Pago])</f>
@@ -3257,9 +3248,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="str">
+      <c r="A7" s="71">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(FatCTL[[#This Row],[0]]=E6,"",FatCTL[[#This Row],[0]]))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="B7" s="68">
         <f>IF(ControleOSsMês!$B$1="Todas",IF(IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")=0,"",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($B$1)-1))+1,1),"")),IFERROR(VLOOKUP(INT((ROW()-ROW($B$1)-1))+1,OSCTL[],2,FALSE),""))</f>
@@ -3267,15 +3258,15 @@
       </c>
       <c r="C7" s="77">
         <f ca="1">IF(FatCTL[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(FatCTL[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(FatCTL[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="D7" s="77">
         <f ca="1">IF(B7="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B7,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="70" t="str">
+        <v>56</v>
+      </c>
+      <c r="E7" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E6,E6+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3295,9 +3286,9 @@
         <f ca="1">IF(B8="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B8,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E8" s="70" t="str">
+      <c r="E8" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E7,E7+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3317,9 +3308,9 @@
         <f ca="1">IF(B9="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B9,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E9" s="70" t="str">
+      <c r="E9" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E8,E8+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3339,9 +3330,9 @@
         <f ca="1">IF(B10="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B10,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B10,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E10" s="70" t="str">
+      <c r="E10" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E9,E9+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3361,9 +3352,9 @@
         <f ca="1">IF(B11="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B11,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B11,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E11" s="70" t="str">
+      <c r="E11" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E10,E10+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3383,9 +3374,9 @@
         <f ca="1">IF(B12="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B12,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B12,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E12" s="70" t="str">
+      <c r="E12" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E11,E11+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3405,9 +3396,9 @@
         <f ca="1">IF(B13="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B13,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B13,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E13" s="70" t="str">
+      <c r="E13" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E12,E12+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3427,9 +3418,9 @@
         <f ca="1">IF(B14="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B14,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B14,Mensal!$A$5:$A$154,0)+4,3)))</f>
         <v>0</v>
       </c>
-      <c r="E14" s="70" t="str">
+      <c r="E14" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E13,E13+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3451,7 +3442,7 @@
       </c>
       <c r="E15" s="70">
         <f ca="1">IF(FatCTL[[#This Row],[Saldo em PF]]=0,E14,E14+1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3468,7 +3459,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3578,7 +3569,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,7 +3677,7 @@
       <c r="A2" s="21">
         <v>4721</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="59" t="s">
         <v>145</v>
       </c>
       <c r="C2" s="50">
@@ -3750,7 +3741,7 @@
       <c r="A3" s="21">
         <v>4757</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="59" t="s">
         <v>145</v>
       </c>
       <c r="C3" s="50">
@@ -3812,11 +3803,11 @@
       <c r="A4" s="21">
         <v>4776</v>
       </c>
-      <c r="B4" t="s">
-        <v>81</v>
+      <c r="B4" s="59" t="s">
+        <v>145</v>
       </c>
       <c r="C4" s="50">
-        <v>42675</v>
+        <v>42679</v>
       </c>
       <c r="D4" t="s">
         <v>96</v>
@@ -3848,7 +3839,7 @@
         <v>94</v>
       </c>
       <c r="O4" s="21">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P4" s="21">
         <v>3</v>
@@ -3868,19 +3859,19 @@
       <c r="W4" s="21"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="21">
-        <f>(VALUE("11/07/16")-VALUE("30/06/16")+1)+(VALUE("17/08/16")-VALUE("18/07/16")+1)+(VALUE("07/09/16")-VALUE("18/08/16")+1)+(VALUE("09/09/16")-VALUE("26/08/16")+1)+(VALUE("15/10/16")-VALUE("16/09/16")+1)</f>
-        <v>109</v>
+        <f>(VALUE("11/07/16")-VALUE("30/06/16")+1)+(VALUE("17/08/16")-VALUE("18/07/16")+1)+(VALUE("07/09/16")-VALUE("18/08/16")+1)+(VALUE("09/09/16")-VALUE("26/08/16")+1)+(VALUE("15/10/16")-VALUE("16/09/16")+1)+(VALUE("15/11/16")-VALUE("07/11/16")+1)</f>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>4777</v>
       </c>
-      <c r="B5" t="s">
-        <v>81</v>
+      <c r="B5" s="59" t="s">
+        <v>145</v>
       </c>
       <c r="C5" s="50">
-        <v>42675</v>
+        <v>42679</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
@@ -3933,19 +3924,19 @@
       <c r="W5" s="21"/>
       <c r="X5" s="21"/>
       <c r="Y5" s="21">
-        <f>(VALUE("09/08/16")-VALUE("20/07/16")+1)+(VALUE("27/09/16")-VALUE("22/08/16")+1)+(VALUE("15/10/16")-VALUE("04/10/16")+1)</f>
-        <v>70</v>
+        <f>(VALUE("09/08/16")-VALUE("20/07/16")+1)+(VALUE("27/09/16")-VALUE("22/08/16")+1)+(VALUE("15/10/16")-VALUE("04/10/16")+1)+(VALUE("15/11/16")-VALUE("07/11/16")+1)</f>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4782</v>
       </c>
-      <c r="B6" t="s">
-        <v>81</v>
+      <c r="B6" s="59" t="s">
+        <v>145</v>
       </c>
       <c r="C6" s="50">
-        <v>42675</v>
+        <v>42682</v>
       </c>
       <c r="D6" t="s">
         <v>96</v>
@@ -3995,16 +3986,16 @@
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
       <c r="Y6" s="21">
-        <f>(VALUE("19/08/16")-VALUE("04/08/16")+1)+(VALUE("13/10/16")-VALUE("15/09/16")+1)</f>
-        <v>45</v>
+        <f>(VALUE("19/08/16")-VALUE("04/08/16")+1)+(VALUE("13/10/16")-VALUE("15/09/16")+1)+(VALUE("15/11/16")-VALUE("09/11/16")+1)</f>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>4797</v>
       </c>
-      <c r="B7" t="s">
-        <v>77</v>
+      <c r="B7" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="C7" s="50">
         <v>42372</v>
@@ -4031,7 +4022,9 @@
       <c r="K7" s="50">
         <v>42677</v>
       </c>
-      <c r="L7" s="50"/>
+      <c r="L7" s="50">
+        <v>42688</v>
+      </c>
       <c r="M7" s="50"/>
       <c r="N7" s="21">
         <v>50</v>
@@ -4059,7 +4052,7 @@
       <c r="A8" s="21">
         <v>4808</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="59" t="s">
         <v>204</v>
       </c>
       <c r="C8" s="50">
@@ -4109,7 +4102,7 @@
       <c r="A9" s="21">
         <v>4809</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="59" t="s">
         <v>145</v>
       </c>
       <c r="C9" s="50">
@@ -4136,7 +4129,7 @@
       <c r="L9" s="50"/>
       <c r="M9" s="50"/>
       <c r="N9" s="21">
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
@@ -4149,15 +4142,15 @@
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="21">
-        <f>(VALUE("31/10/16")-VALUE("22/08/16")+1)</f>
-        <v>71</v>
+        <f>(VALUE("15/11/16")-VALUE("22/08/16")+1)</f>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>4810</v>
       </c>
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="59" t="s">
         <v>145</v>
       </c>
       <c r="C10" s="50">
@@ -4217,7 +4210,7 @@
       <c r="A11" s="21">
         <v>4813</v>
       </c>
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="59" t="s">
         <v>204</v>
       </c>
       <c r="C11" s="50">
@@ -4267,11 +4260,11 @@
       <c r="A12" s="21">
         <v>4817</v>
       </c>
-      <c r="B12" t="s">
-        <v>74</v>
+      <c r="B12" s="59" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="50">
-        <v>42677</v>
+        <v>42684</v>
       </c>
       <c r="D12" t="s">
         <v>96</v>
@@ -4285,9 +4278,13 @@
       <c r="G12" s="50">
         <v>42677</v>
       </c>
-      <c r="H12" s="50"/>
+      <c r="H12" s="50">
+        <v>42684</v>
+      </c>
       <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="J12" s="50">
+        <v>42691</v>
+      </c>
       <c r="K12" s="50"/>
       <c r="L12" s="50"/>
       <c r="M12" s="50"/>
@@ -4310,11 +4307,11 @@
       <c r="A13" s="21">
         <v>4818</v>
       </c>
-      <c r="B13" t="s">
-        <v>74</v>
+      <c r="B13" s="59" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="50">
-        <v>42677</v>
+        <v>42684</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -4328,9 +4325,13 @@
       <c r="G13" s="50">
         <v>42677</v>
       </c>
-      <c r="H13" s="50"/>
+      <c r="H13" s="50">
+        <v>42684</v>
+      </c>
       <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
+      <c r="J13" s="50">
+        <v>42695</v>
+      </c>
       <c r="K13" s="50"/>
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
@@ -4353,11 +4354,11 @@
       <c r="A14" s="21">
         <v>4819</v>
       </c>
-      <c r="B14" t="s">
-        <v>74</v>
+      <c r="B14" s="59" t="s">
+        <v>75</v>
       </c>
       <c r="C14" s="50">
-        <v>42688</v>
+        <v>42695</v>
       </c>
       <c r="D14" t="s">
         <v>96</v>
@@ -4371,7 +4372,9 @@
       <c r="G14" s="50">
         <v>42688</v>
       </c>
-      <c r="H14" s="50"/>
+      <c r="H14" s="50">
+        <v>42695</v>
+      </c>
       <c r="I14" s="50"/>
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
@@ -4431,11 +4434,11 @@
   </sheetPr>
   <dimension ref="A1:AG154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L49" sqref="L49"/>
+      <selection pane="bottomRight" activeCell="A150" sqref="A150:XFD154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4466,7 +4469,7 @@
         <v>119</v>
       </c>
       <c r="B1" s="61">
-        <v>42674</v>
+        <v>42689</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="62" t="s">
@@ -4500,7 +4503,7 @@
       <c r="AE2" s="21"/>
       <c r="AG2" s="51" t="str">
         <f ca="1">IF(ControleOSsMês!$B$1="Todas","Ref. Todas as OS","Ref. "&amp;UPPER(TEXT(ControleOSsMês!$F$1,"MMM/AAAA")))</f>
-        <v>Ref. OUT/2016</v>
+        <v>Ref. NOV/2016</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -4600,7 +4603,7 @@
       </c>
       <c r="C4" s="78">
         <f ca="1">SUM(C5:C154)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="27"/>
@@ -5035,8 +5038,14 @@
       </c>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="35"/>
+      <c r="O9" s="76" t="str">
+        <f>IF(P9="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P9" s="21" t="str">
+        <f>IF(A5="","",IF(VLOOKUP(A5,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A5,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="52">
@@ -5056,7 +5065,7 @@
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42644</v>
       </c>
-      <c r="F10" s="112" t="str">
+      <c r="F10" s="113" t="str">
         <f>IF(A10="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -5073,7 +5082,7 @@
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
-      <c r="Q10" s="112" t="str">
+      <c r="Q10" s="113" t="str">
         <f>IF(A10="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -5458,8 +5467,14 @@
       </c>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="35"/>
+      <c r="O14" s="76" t="str">
+        <f>IF(P14="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P14" s="21" t="str">
+        <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="52">
@@ -5468,7 +5483,7 @@
       </c>
       <c r="B15" s="114" t="str">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Devolvida</v>
+        <v>Paralisada</v>
       </c>
       <c r="C15" s="114"/>
       <c r="D15" s="52" t="str">
@@ -5477,9 +5492,9 @@
       </c>
       <c r="E15" s="56">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
-      </c>
-      <c r="F15" s="112" t="str">
+        <v>42679</v>
+      </c>
+      <c r="F15" s="113" t="str">
         <f>IF(A15="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -5496,7 +5511,7 @@
       <c r="N15" s="28"/>
       <c r="O15" s="28"/>
       <c r="P15" s="28"/>
-      <c r="Q15" s="112" t="str">
+      <c r="Q15" s="113" t="str">
         <f>IF(A15="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -5550,27 +5565,27 @@
       </c>
       <c r="I16" s="20">
         <f>IF(G16="","",G16+ROUND(((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42671</v>
+        <v>42679</v>
       </c>
       <c r="J16" s="20">
         <f>IF(I16="","",WORKDAY(IF(I17="",I16,IF(I17&gt;I16,I17,I16)),IF(IF(P17="",P16,P17)&lt;150,5,10)))</f>
-        <v>42678</v>
+        <v>42685</v>
       </c>
       <c r="K16" s="20">
         <f>IF(J16="","",J16+ROUND((IF(P17="",P16,IF(P17&gt;P16,P17,P16))/(19*LN(IF(P17="",P16,IF(P17&gt;P16,P17,P16)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42692</v>
+        <v>42698</v>
       </c>
       <c r="L16" s="20">
         <f>IF(G16="","",G16+ROUND(((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42699</v>
+        <v>42706</v>
       </c>
       <c r="M16" s="20">
         <f>IF(K16="","",WORKDAY(K16,1))</f>
-        <v>42695</v>
+        <v>42699</v>
       </c>
       <c r="N16" s="20">
         <f>IF(M16="","",M16+SLA_PrazoGarantia)</f>
-        <v>42875</v>
+        <v>42879</v>
       </c>
       <c r="O16" s="27" t="str">
         <f>IF(A15="","","Previsto")</f>
@@ -5582,7 +5597,7 @@
       </c>
       <c r="Q16" s="54">
         <f>IF(F16="","",ROUND((L16-G16)*SLA_ICP_EOS,1))</f>
-        <v>17.8</v>
+        <v>18.5</v>
       </c>
       <c r="R16" s="21">
         <f>IF(F16="","",SLA_ICP_CIHA)</f>
@@ -5618,7 +5633,7 @@
       </c>
       <c r="Z16" s="54">
         <f>IF(F16="","",ROUND((L16-G16)*SLA_ICA_EOS,1))</f>
-        <v>44.5</v>
+        <v>46.3</v>
       </c>
       <c r="AA16" t="str">
         <f>IF(A15="","","Homologação")</f>
@@ -5638,7 +5653,7 @@
       </c>
       <c r="AE16" s="24">
         <f>IF(A15="","",AD16/IF($P17="",$P16,$P17))</f>
-        <v>0.14018691588785046</v>
+        <v>0.14423076923076922</v>
       </c>
       <c r="AF16" s="21">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Atrasos para Correção Homologação",OSS[#Headers],0),FALSE))</f>
@@ -5699,7 +5714,7 @@
         <f>IF(A15="","",IF(VLOOKUP(A15,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A15,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)
 +IF(VLOOKUP(A15,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))
 ))</f>
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q17" s="54">
         <f ca="1">IF(F16="","",IF(G17="","",IF(L17="",IF(DataRef&lt;L16,L16,DataRef),L17)-L16))</f>
@@ -5719,7 +5734,7 @@
       </c>
       <c r="U17" s="24">
         <f>IF(J17="","",AC16/IF($P17="",$P16,$P17))</f>
-        <v>0.14018691588785046</v>
+        <v>0.14423076923076922</v>
       </c>
       <c r="V17" s="24" t="str">
         <f>IF(K17="","",AB17/IF($P17="",$P16,$P17))</f>
@@ -5774,7 +5789,7 @@
       <c r="C18" s="82"/>
       <c r="D18" s="81">
         <f ca="1">IF(A15="","",P18)</f>
-        <v>-9.6999999999999993</v>
+        <v>-9.8000000000000007</v>
       </c>
       <c r="E18" s="35"/>
       <c r="K18" s="64" t="str">
@@ -5783,7 +5798,7 @@
       </c>
       <c r="L18" s="65">
         <f>IF(G16="","",ROUND((IF(P17="",P16,P17)/(19*LN(IF(P17="",P16,P17))-42))*30,0)+IF(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="O18" s="27" t="str">
         <f>IF(A15="","","Multa")</f>
@@ -5791,7 +5806,7 @@
       </c>
       <c r="P18" s="54">
         <f ca="1">IF(SUM(Q18:Z18)=0,"",-ROUND(SUM(Q18:Z18),1))</f>
-        <v>-9.6999999999999993</v>
+        <v>-9.8000000000000007</v>
       </c>
       <c r="Q18" s="54" t="str">
         <f ca="1">IF(Q17="","",IF(OR(Q16&gt;Q17,Z16&lt;Z17),"",ROUND(Q17*(IF($P17="",$P16,$P17)*SLA_ICP_EOS_Multa),2)))</f>
@@ -5811,7 +5826,7 @@
       </c>
       <c r="U18" s="54">
         <f>IF(U17="","",IF(U16&gt;U17,"",ROUND((U17-U16)*100*(IF($P17="",$P16,$P17)*SLA_IQA_IGHA_Multa),2)))</f>
-        <v>9.65</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="V18" s="54" t="str">
         <f>IF(V17="","",IF(V16&gt;V17,"",ROUND((V17-V16)*100*(IF($P17="",$P16,$P17)*SLA_IQA_INGG_Multa),2)))</f>
@@ -5851,7 +5866,7 @@
       </c>
       <c r="AE18" s="24">
         <f>IF(P16="","",IF(AD18="","",AD18/IF($P17="",$P16,$P17)))</f>
-        <v>0.14018691588785046</v>
+        <v>0.14423076923076922</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
@@ -5865,7 +5880,7 @@
       </c>
       <c r="D19" s="81">
         <f ca="1">IF(P16="","",IF($P17="",$P16,$P17)+IF(D18="",0,D18)-IF(D17="",0,D17))</f>
-        <v>14.099999999999994</v>
+        <v>11</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -5877,12 +5892,18 @@
       </c>
       <c r="L19" s="65">
         <f>IF(G16="","",IF(IFERROR(VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A15,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="35"/>
+      <c r="O19" s="76" t="str">
+        <f>IF(P19="","","Alteração")</f>
+        <v>Alteração</v>
+      </c>
+      <c r="P19" s="21">
+        <f>IF(A15="","",IF(VLOOKUP(A15,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A15,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="52">
@@ -5891,7 +5912,7 @@
       </c>
       <c r="B20" s="114" t="str">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Devolvida</v>
+        <v>Paralisada</v>
       </c>
       <c r="C20" s="114"/>
       <c r="D20" s="52" t="str">
@@ -5900,9 +5921,9 @@
       </c>
       <c r="E20" s="56">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
-      </c>
-      <c r="F20" s="112" t="str">
+        <v>42679</v>
+      </c>
+      <c r="F20" s="113" t="str">
         <f>IF(A20="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -5919,7 +5940,7 @@
       <c r="N20" s="28"/>
       <c r="O20" s="28"/>
       <c r="P20" s="28"/>
-      <c r="Q20" s="112" t="str">
+      <c r="Q20" s="113" t="str">
         <f>IF(A20="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -5973,27 +5994,27 @@
       </c>
       <c r="I21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42653</v>
+        <v>42662</v>
       </c>
       <c r="J21" s="20">
         <f>IF(I21="","",WORKDAY(IF(I22="",I21,IF(I22&gt;I21,I22,I21)),IF(IF(P22="",P21,P22)&lt;150,5,10)))</f>
-        <v>42667</v>
+        <v>42676</v>
       </c>
       <c r="K21" s="20">
         <f>IF(J21="","",J21+ROUND((IF(P22="",P21,IF(P22&gt;P21,P22,P21))/(19*LN(IF(P22="",P21,IF(P22&gt;P21,P22,P21)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42685</v>
+        <v>42694</v>
       </c>
       <c r="L21" s="20">
         <f>IF(G21="","",G21+ROUND(((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42689</v>
+        <v>42698</v>
       </c>
       <c r="M21" s="20">
         <f>IF(K21="","",WORKDAY(K21,1))</f>
-        <v>42688</v>
+        <v>42695</v>
       </c>
       <c r="N21" s="20">
         <f>IF(M21="","",M21+SLA_PrazoGarantia)</f>
-        <v>42868</v>
+        <v>42875</v>
       </c>
       <c r="O21" s="27" t="str">
         <f>IF(A20="","","Previsto")</f>
@@ -6005,7 +6026,7 @@
       </c>
       <c r="Q21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICP_EOS,1))</f>
-        <v>16.100000000000001</v>
+        <v>17</v>
       </c>
       <c r="R21" s="21">
         <f>IF(F21="","",SLA_ICP_CIHA)</f>
@@ -6041,7 +6062,7 @@
       </c>
       <c r="Z21" s="54">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICA_EOS,1))</f>
-        <v>40.299999999999997</v>
+        <v>42.5</v>
       </c>
       <c r="AA21" t="str">
         <f>IF(A20="","","Homologação")</f>
@@ -6206,7 +6227,7 @@
       </c>
       <c r="L23" s="65">
         <f>IF(G21="","",ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30,0)+IF(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="O23" s="27" t="str">
         <f>IF(A20="","","Multa")</f>
@@ -6300,12 +6321,18 @@
       </c>
       <c r="L24" s="65">
         <f>IF(G21="","",IF(IFERROR(VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A20,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="35"/>
+      <c r="O24" s="76" t="str">
+        <f>IF(P24="","","Alteração")</f>
+        <v>Alteração</v>
+      </c>
+      <c r="P24" s="21">
+        <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v>15.5</v>
+      </c>
     </row>
     <row r="25" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="52">
@@ -6314,7 +6341,7 @@
       </c>
       <c r="B25" s="114" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Devolvida</v>
+        <v>Paralisada</v>
       </c>
       <c r="C25" s="114"/>
       <c r="D25" s="52" t="str">
@@ -6323,9 +6350,9 @@
       </c>
       <c r="E25" s="56">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
-      </c>
-      <c r="F25" s="112" t="str">
+        <v>42682</v>
+      </c>
+      <c r="F25" s="113" t="str">
         <f>IF(A25="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -6342,7 +6369,7 @@
       <c r="N25" s="28"/>
       <c r="O25" s="28"/>
       <c r="P25" s="28"/>
-      <c r="Q25" s="112" t="str">
+      <c r="Q25" s="113" t="str">
         <f>IF(A25="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -6396,7 +6423,7 @@
       </c>
       <c r="I26" s="20">
         <f>IF(G26="","",G26+ROUND(((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42634</v>
+        <v>42641</v>
       </c>
       <c r="J26" s="20">
         <f>IF(I26="","",WORKDAY(IF(I27="",I26,IF(I27&gt;I26,I27,I26)),IF(IF(P27="",P26,P27)&lt;150,5,10)))</f>
@@ -6408,7 +6435,7 @@
       </c>
       <c r="L26" s="20">
         <f>IF(G26="","",G26+ROUND(((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42669</v>
+        <v>42676</v>
       </c>
       <c r="M26" s="20">
         <f>IF(K26="","",WORKDAY(K26,1))</f>
@@ -6428,7 +6455,7 @@
       </c>
       <c r="Q26" s="54">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICP_EOS,1))</f>
-        <v>13.3</v>
+        <v>14</v>
       </c>
       <c r="R26" s="21">
         <f>IF(F26="","",SLA_ICP_CIHA)</f>
@@ -6464,7 +6491,7 @@
       </c>
       <c r="Z26" s="54">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICA_EOS,1))</f>
-        <v>33.299999999999997</v>
+        <v>35</v>
       </c>
       <c r="AA26" t="str">
         <f>IF(A25="","","Homologação")</f>
@@ -6549,7 +6576,7 @@
       </c>
       <c r="Q27" s="54">
         <f ca="1">IF(F26="","",IF(G27="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="R27" s="21">
         <f>IF(J27="","",AF26)</f>
@@ -6585,7 +6612,7 @@
       </c>
       <c r="Z27" s="54">
         <f ca="1">IF(F26="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AA27" t="str">
         <f>IF(A25="","","Garantia")</f>
@@ -6629,7 +6656,7 @@
       </c>
       <c r="L28" s="65">
         <f>IF(G26="","",ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30,0)+IF(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="O28" s="27" t="str">
         <f>IF(A25="","","Multa")</f>
@@ -6723,12 +6750,18 @@
       </c>
       <c r="L29" s="65">
         <f>IF(G26="","",IF(IFERROR(VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A25,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="M29" s="20"/>
       <c r="N29" s="20"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="35"/>
+      <c r="O29" s="76" t="str">
+        <f>IF(P29="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P29" s="21" t="str">
+        <f>IF(A25="","",IF(VLOOKUP(A25,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A25,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="52">
@@ -6737,7 +6770,7 @@
       </c>
       <c r="B30" s="114" t="str">
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Entregue</v>
+        <v>Recebida</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="52" t="str">
@@ -6748,7 +6781,7 @@
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42372</v>
       </c>
-      <c r="F30" s="112" t="str">
+      <c r="F30" s="113" t="str">
         <f>IF(A30="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -6765,7 +6798,7 @@
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
-      <c r="Q30" s="112" t="str">
+      <c r="Q30" s="113" t="str">
         <f>IF(A30="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -6799,11 +6832,11 @@
       </c>
       <c r="D31" s="81">
         <f ca="1">IF(E31="","",ROUND(IF($P32="",$P31,$P32)*E31,1))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="E31" s="87">
         <f ca="1">IF(A30="","",IF(D34&lt;0,0,IF(B30="Recebida",0.8,IF(B30="Aceita",0.2,0))))</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F31" s="34">
         <f>IF(A30="","",VLOOKUP(A30,OSS[],MATCH("Abertura da OS",OSS[#Headers],0),FALSE))</f>
@@ -6940,9 +6973,9 @@
         <f>IF(A30="","",IF(VLOOKUP(A30,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A30,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
         <v>42677</v>
       </c>
-      <c r="J32" s="20" t="str">
+      <c r="J32" s="20">
         <f>IF(A30="","",IF(VLOOKUP(A30,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A30,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42688</v>
       </c>
       <c r="K32" s="20" t="str">
         <f>IF(A30="","",IF(VLOOKUP(A30,OSS[],MATCH("Aceite da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A30,OSS[],MATCH("Aceite da OS",OSS[#Headers],0),FALSE)))</f>
@@ -6974,21 +7007,21 @@
         <f ca="1">IF(F31="","",IF(G32="","",IF(L32="",IF(DataRef&lt;L31,L31,DataRef),L32)-L31))</f>
         <v>0</v>
       </c>
-      <c r="R32" s="21" t="str">
+      <c r="R32" s="21">
         <f>IF(J32="","",AF31)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S32" s="21" t="str">
         <f>IF(K32="","",AF32)</f>
         <v/>
       </c>
-      <c r="T32" s="24" t="str">
+      <c r="T32" s="24">
         <f>IF(J32="","",AB31/IF($P32="",$P31,$P32))</f>
-        <v/>
-      </c>
-      <c r="U32" s="24" t="str">
+        <v>0</v>
+      </c>
+      <c r="U32" s="24">
         <f>IF(J32="","",AC31/IF($P32="",$P31,$P32))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="V32" s="24" t="str">
         <f>IF(K32="","",AB32/IF($P32="",$P31,$P32))</f>
@@ -7130,7 +7163,7 @@
       </c>
       <c r="C34" s="88">
         <f ca="1">IF(A30="","",IF(D34&lt;0,D34,IF(D31=0,0,IF(D31&gt;D34,D31-D34,D31))))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="D34" s="81">
         <f ca="1">IF(P31="","",IF($P32="",$P31,$P32)+IF(D33="",0,D33)-IF(D32="",0,D32))</f>
@@ -7150,8 +7183,14 @@
       </c>
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="35"/>
+      <c r="O34" s="76" t="str">
+        <f>IF(P34="","","Alteração")</f>
+        <v>Alteração</v>
+      </c>
+      <c r="P34" s="21">
+        <f>IF(A30="","",IF(VLOOKUP(A30,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A30,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="35" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="52">
@@ -7171,7 +7210,7 @@
         <f>IF(A35="","",VLOOKUP(A35,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42642</v>
       </c>
-      <c r="F35" s="112" t="str">
+      <c r="F35" s="113" t="str">
         <f>IF(A35="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -7188,7 +7227,7 @@
       <c r="N35" s="28"/>
       <c r="O35" s="28"/>
       <c r="P35" s="28"/>
-      <c r="Q35" s="112" t="str">
+      <c r="Q35" s="113" t="str">
         <f>IF(A35="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -7573,8 +7612,14 @@
       </c>
       <c r="M39" s="20"/>
       <c r="N39" s="20"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="35"/>
+      <c r="O39" s="76" t="str">
+        <f>IF(P39="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P39" s="21" t="str">
+        <f>IF(A35="","",IF(VLOOKUP(A35,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A35,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="52">
@@ -7594,7 +7639,7 @@
         <f>IF(A40="","",VLOOKUP(A40,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42604</v>
       </c>
-      <c r="F40" s="112" t="str">
+      <c r="F40" s="113" t="str">
         <f>IF(A40="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -7611,7 +7656,7 @@
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
       <c r="P40" s="28"/>
-      <c r="Q40" s="112" t="str">
+      <c r="Q40" s="113" t="str">
         <f>IF(A40="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -7657,35 +7702,35 @@
       </c>
       <c r="G41" s="20">
         <f>IF(F41="","",WORKDAY(F41,IF(IF(P42="",P41,P42)&lt;150,5,10)))</f>
-        <v>42605</v>
+        <v>42598</v>
       </c>
       <c r="H41" s="20">
         <f>IF(G41="","",WORKDAY(G41,5))</f>
-        <v>42612</v>
+        <v>42605</v>
       </c>
       <c r="I41" s="20">
         <f>IF(G41="","",G41+ROUND(((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42742</v>
+        <v>42727</v>
       </c>
       <c r="J41" s="20">
         <f>IF(I41="","",WORKDAY(IF(I42="",I41,IF(I42&gt;I41,I42,I41)),IF(IF(P42="",P41,P42)&lt;150,5,10)))</f>
-        <v>42755</v>
+        <v>42734</v>
       </c>
       <c r="K41" s="20">
         <f>IF(J41="","",J41+ROUND((IF(P42="",P41,IF(P42&gt;P41,P42,P41))/(19*LN(IF(P42="",P41,IF(P42&gt;P41,P42,P41)))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42777</v>
+        <v>42748</v>
       </c>
       <c r="L41" s="20">
         <f>IF(G41="","",G41+ROUND(((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42786</v>
+        <v>42756</v>
       </c>
       <c r="M41" s="20">
         <f>IF(K41="","",WORKDAY(K41,1))</f>
-        <v>42779</v>
+        <v>42751</v>
       </c>
       <c r="N41" s="20">
         <f>IF(M41="","",M41+SLA_PrazoGarantia)</f>
-        <v>42959</v>
+        <v>42931</v>
       </c>
       <c r="O41" s="27" t="str">
         <f>IF(A40="","","Previsto")</f>
@@ -7693,11 +7738,11 @@
       </c>
       <c r="P41" s="21">
         <f>IF(A40="","",VLOOKUP(A40,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE))</f>
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="Q41" s="54">
         <f>IF(F41="","",ROUND((L41-G41)*SLA_ICP_EOS,1))</f>
-        <v>18.100000000000001</v>
+        <v>15.8</v>
       </c>
       <c r="R41" s="21">
         <f>IF(F41="","",SLA_ICP_CIHA)</f>
@@ -7725,7 +7770,7 @@
       </c>
       <c r="X41" s="54">
         <f>IF(F41="","",ROUND((G41-F41)*SLA_ICA_IOS,1))</f>
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
       <c r="Y41" s="54" t="str">
         <f>IF(OR(R40="Hora Java",R40="Hora dotNet"),SLA_ICA_SP,"")</f>
@@ -7733,7 +7778,7 @@
       </c>
       <c r="Z41" s="54">
         <f>IF(F41="","",ROUND((L41-G41)*SLA_ICA_EOS,1))</f>
-        <v>45.3</v>
+        <v>39.5</v>
       </c>
       <c r="AA41" t="str">
         <f>IF(A40="","","Homologação")</f>
@@ -7898,7 +7943,7 @@
       </c>
       <c r="L43" s="65">
         <f>IF(G41="","",ROUND((IF(P42="",P41,P42)/(19*LN(IF(P42="",P41,P42))-42))*30,0)+IF(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="O43" s="27" t="str">
         <f>IF(A40="","","Multa")</f>
@@ -7980,7 +8025,7 @@
       </c>
       <c r="D44" s="81">
         <f ca="1">IF(P41="","",IF($P42="",$P41,$P42)+IF(D43="",0,D43)-IF(D42="",0,D42))</f>
-        <v>224</v>
+        <v>117</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="20"/>
@@ -7992,12 +8037,18 @@
       </c>
       <c r="L44" s="65">
         <f>IF(G41="","",IF(IFERROR(VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(A40,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="20"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="35"/>
+      <c r="O44" s="76" t="str">
+        <f>IF(P44="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P44" s="21" t="str">
+        <f>IF(A40="","",IF(VLOOKUP(A40,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A40,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="52">
@@ -8017,7 +8068,7 @@
         <f>IF(A45="","",VLOOKUP(A45,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42646</v>
       </c>
-      <c r="F45" s="112" t="str">
+      <c r="F45" s="113" t="str">
         <f>IF(A45="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -8034,7 +8085,7 @@
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
       <c r="P45" s="28"/>
-      <c r="Q45" s="112" t="str">
+      <c r="Q45" s="113" t="str">
         <f>IF(A45="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -8419,8 +8470,14 @@
       </c>
       <c r="M49" s="20"/>
       <c r="N49" s="20"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="35"/>
+      <c r="O49" s="76" t="str">
+        <f>IF(P49="","","Alteração")</f>
+        <v>Alteração</v>
+      </c>
+      <c r="P49" s="21">
+        <f>IF(A45="","",IF(VLOOKUP(A45,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A45,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="50" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="52">
@@ -8440,7 +8497,7 @@
         <f>IF(A50="","",VLOOKUP(A50,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42647</v>
       </c>
-      <c r="F50" s="112" t="str">
+      <c r="F50" s="113" t="str">
         <f>IF(A50="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -8457,7 +8514,7 @@
       <c r="N50" s="28"/>
       <c r="O50" s="28"/>
       <c r="P50" s="28"/>
-      <c r="Q50" s="112" t="str">
+      <c r="Q50" s="113" t="str">
         <f>IF(A50="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -8842,8 +8899,14 @@
       </c>
       <c r="M54" s="20"/>
       <c r="N54" s="20"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="35"/>
+      <c r="O54" s="76" t="str">
+        <f>IF(P54="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P54" s="21" t="str">
+        <f>IF(A50="","",IF(VLOOKUP(A50,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A50,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="55" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="52">
@@ -8852,7 +8915,7 @@
       </c>
       <c r="B55" s="114" t="str">
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Iniciada</v>
       </c>
       <c r="C55" s="114"/>
       <c r="D55" s="52" t="str">
@@ -8861,9 +8924,9 @@
       </c>
       <c r="E55" s="56">
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42677</v>
-      </c>
-      <c r="F55" s="112" t="str">
+        <v>42684</v>
+      </c>
+      <c r="F55" s="113" t="str">
         <f>IF(A55="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -8880,7 +8943,7 @@
       <c r="N55" s="28"/>
       <c r="O55" s="28"/>
       <c r="P55" s="28"/>
-      <c r="Q55" s="112" t="str">
+      <c r="Q55" s="113" t="str">
         <f>IF(A55="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -9043,13 +9106,13 @@
         <f>IF(A55="","",VLOOKUP(A55,OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE))</f>
         <v>0</v>
       </c>
-      <c r="G57" s="20" t="str">
+      <c r="G57" s="20">
         <f>IF(A55="","",IF(VLOOKUP(A55,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A55,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H57" s="20" t="str">
+        <v>42684</v>
+      </c>
+      <c r="H57" s="20">
         <f>IF(A55="","",IF(VLOOKUP(A55,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A55,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42691</v>
       </c>
       <c r="I57" s="20" t="str">
         <f>IF(A55="","",IF(VLOOKUP(A55,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A55,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
@@ -9085,9 +9148,9 @@
 ))</f>
         <v/>
       </c>
-      <c r="Q57" s="54" t="str">
-        <f>IF(F56="","",IF(G57="","",IF(L57="",IF(DataRef&lt;L56,L56,DataRef),L57)-L56))</f>
-        <v/>
+      <c r="Q57" s="54">
+        <f ca="1">IF(F56="","",IF(G57="","",IF(L57="",IF(DataRef&lt;L56,L56,DataRef),L57)-L56))</f>
+        <v>0</v>
       </c>
       <c r="R57" s="21" t="str">
         <f>IF(J57="","",AF56)</f>
@@ -9113,9 +9176,9 @@
         <f>IF(K57="","",AC57/IF($P57="",$P56,$P57))</f>
         <v/>
       </c>
-      <c r="X57" s="54" t="str">
-        <f ca="1">IF(F56="","",IF(G57="",IF(DataRef&lt;G56,"",DataRef-G56),IF(G57&lt;G56,"",G57-G56)))</f>
-        <v/>
+      <c r="X57" s="54">
+        <f>IF(F56="","",IF(G57="",IF(DataRef&lt;G56,"",DataRef-G56),IF(G57&lt;G56,"",G57-G56)))</f>
+        <v>0</v>
       </c>
       <c r="Y57" s="54" t="str">
         <f>IF(OR(R55="Hora Java",R55="Hora dotNet"),AG56,"")</f>
@@ -9178,7 +9241,7 @@
         <v/>
       </c>
       <c r="Q58" s="54" t="str">
-        <f>IF(Q57="","",IF(OR(Q56&gt;Q57,Z56&lt;Z57),"",ROUND(Q57*(IF($P57="",$P56,$P57)*SLA_ICP_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q57="","",IF(OR(Q56&gt;Q57,Z56&lt;Z57),"",ROUND(Q57*(IF($P57="",$P56,$P57)*SLA_ICP_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R58" s="54" t="str">
@@ -9206,7 +9269,7 @@
         <v/>
       </c>
       <c r="X58" s="54" t="str">
-        <f ca="1">IF(X57="","",IF(X56&gt;X57,"",ROUND(X57*(IF($P57="",$P56,$P57)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X57="","",IF(X56&gt;X57,"",ROUND(X57*(IF($P57="",$P56,$P57)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y58" s="54" t="str">
@@ -9265,8 +9328,14 @@
       </c>
       <c r="M59" s="20"/>
       <c r="N59" s="20"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="35"/>
+      <c r="O59" s="76" t="str">
+        <f>IF(P59="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P59" s="21" t="str">
+        <f>IF(A55="","",IF(VLOOKUP(A55,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A55,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="60" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="52">
@@ -9275,7 +9344,7 @@
       </c>
       <c r="B60" s="114" t="str">
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Iniciada</v>
       </c>
       <c r="C60" s="114"/>
       <c r="D60" s="52" t="str">
@@ -9284,9 +9353,9 @@
       </c>
       <c r="E60" s="56">
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42677</v>
-      </c>
-      <c r="F60" s="112" t="str">
+        <v>42684</v>
+      </c>
+      <c r="F60" s="113" t="str">
         <f>IF(A60="","","Titulo:")</f>
         <v>Titulo:</v>
       </c>
@@ -9303,7 +9372,7 @@
       <c r="N60" s="28"/>
       <c r="O60" s="28"/>
       <c r="P60" s="28"/>
-      <c r="Q60" s="112" t="str">
+      <c r="Q60" s="113" t="str">
         <f>IF(A60="","","Tipo da OS:")</f>
         <v>Tipo da OS:</v>
       </c>
@@ -9466,13 +9535,13 @@
         <f>IF(A60="","",VLOOKUP(A60,OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE))</f>
         <v>0</v>
       </c>
-      <c r="G62" s="20" t="str">
+      <c r="G62" s="20">
         <f>IF(A60="","",IF(VLOOKUP(A60,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A60,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
-      </c>
-      <c r="H62" s="20" t="str">
+        <v>42684</v>
+      </c>
+      <c r="H62" s="20">
         <f>IF(A60="","",IF(VLOOKUP(A60,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A60,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42695</v>
       </c>
       <c r="I62" s="20" t="str">
         <f>IF(A60="","",IF(VLOOKUP(A60,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A60,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
@@ -9508,9 +9577,9 @@
 ))</f>
         <v/>
       </c>
-      <c r="Q62" s="54" t="str">
-        <f>IF(F61="","",IF(G62="","",IF(L62="",IF(DataRef&lt;L61,L61,DataRef),L62)-L61))</f>
-        <v/>
+      <c r="Q62" s="54">
+        <f ca="1">IF(F61="","",IF(G62="","",IF(L62="",IF(DataRef&lt;L61,L61,DataRef),L62)-L61))</f>
+        <v>0</v>
       </c>
       <c r="R62" s="21" t="str">
         <f>IF(J62="","",AF61)</f>
@@ -9536,9 +9605,9 @@
         <f>IF(K62="","",AC62/IF($P62="",$P61,$P62))</f>
         <v/>
       </c>
-      <c r="X62" s="54" t="str">
-        <f ca="1">IF(F61="","",IF(G62="",IF(DataRef&lt;G61,"",DataRef-G61),IF(G62&lt;G61,"",G62-G61)))</f>
-        <v/>
+      <c r="X62" s="54">
+        <f>IF(F61="","",IF(G62="",IF(DataRef&lt;G61,"",DataRef-G61),IF(G62&lt;G61,"",G62-G61)))</f>
+        <v>0</v>
       </c>
       <c r="Y62" s="54" t="str">
         <f>IF(OR(R60="Hora Java",R60="Hora dotNet"),AG61,"")</f>
@@ -9601,7 +9670,7 @@
         <v/>
       </c>
       <c r="Q63" s="54" t="str">
-        <f>IF(Q62="","",IF(OR(Q61&gt;Q62,Z61&lt;Z62),"",ROUND(Q62*(IF($P62="",$P61,$P62)*SLA_ICP_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q62="","",IF(OR(Q61&gt;Q62,Z61&lt;Z62),"",ROUND(Q62*(IF($P62="",$P61,$P62)*SLA_ICP_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R63" s="54" t="str">
@@ -9629,7 +9698,7 @@
         <v/>
       </c>
       <c r="X63" s="54" t="str">
-        <f ca="1">IF(X62="","",IF(X61&gt;X62,"",ROUND(X62*(IF($P62="",$P61,$P62)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X62="","",IF(X61&gt;X62,"",ROUND(X62*(IF($P62="",$P61,$P62)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y63" s="54" t="str">
@@ -9688,8 +9757,14 @@
       </c>
       <c r="M64" s="20"/>
       <c r="N64" s="20"/>
-      <c r="O64" s="33"/>
-      <c r="P64" s="35"/>
+      <c r="O64" s="76" t="str">
+        <f>IF(P64="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P64" s="21" t="str">
+        <f>IF(A60="","",IF(VLOOKUP(A60,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A60,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="65" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="52">
@@ -9698,7 +9773,7 @@
       </c>
       <c r="B65" s="114" t="str">
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Iniciada</v>
       </c>
       <c r="C65" s="114"/>
       <c r="D65" s="52" t="str">
@@ -9707,7 +9782,7 @@
       </c>
       <c r="E65" s="56">
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42688</v>
+        <v>42695</v>
       </c>
       <c r="F65" s="113" t="str">
         <f>IF(A65="","","Titulo:")</f>
@@ -9889,9 +9964,9 @@
         <f>IF(A65="","",VLOOKUP(A65,OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE))</f>
         <v>0</v>
       </c>
-      <c r="G67" s="20" t="str">
+      <c r="G67" s="20">
         <f>IF(A65="","",IF(VLOOKUP(A65,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A65,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42695</v>
       </c>
       <c r="H67" s="20" t="str">
         <f>IF(A65="","",IF(VLOOKUP(A65,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A65,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
@@ -9931,9 +10006,9 @@
 ))</f>
         <v/>
       </c>
-      <c r="Q67" s="54" t="str">
-        <f>IF(F66="","",IF(G67="","",IF(L67="",IF(DataRef&lt;L66,L66,DataRef),L67)-L66))</f>
-        <v/>
+      <c r="Q67" s="54">
+        <f ca="1">IF(F66="","",IF(G67="","",IF(L67="",IF(DataRef&lt;L66,L66,DataRef),L67)-L66))</f>
+        <v>0</v>
       </c>
       <c r="R67" s="21" t="str">
         <f>IF(J67="","",AF66)</f>
@@ -9959,9 +10034,9 @@
         <f>IF(K67="","",AC67/IF($P67="",$P66,$P67))</f>
         <v/>
       </c>
-      <c r="X67" s="54" t="str">
-        <f ca="1">IF(F66="","",IF(G67="",IF(DataRef&lt;G66,"",DataRef-G66),IF(G67&lt;G66,"",G67-G66)))</f>
-        <v/>
+      <c r="X67" s="54">
+        <f>IF(F66="","",IF(G67="",IF(DataRef&lt;G66,"",DataRef-G66),IF(G67&lt;G66,"",G67-G66)))</f>
+        <v>0</v>
       </c>
       <c r="Y67" s="54" t="str">
         <f>IF(OR(R65="Hora Java",R65="Hora dotNet"),AG66,"")</f>
@@ -10024,7 +10099,7 @@
         <v/>
       </c>
       <c r="Q68" s="54" t="str">
-        <f>IF(Q67="","",IF(OR(Q66&gt;Q67,Z66&lt;Z67),"",ROUND(Q67*(IF($P67="",$P66,$P67)*SLA_ICP_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q67="","",IF(OR(Q66&gt;Q67,Z66&lt;Z67),"",ROUND(Q67*(IF($P67="",$P66,$P67)*SLA_ICP_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R68" s="54" t="str">
@@ -10052,7 +10127,7 @@
         <v/>
       </c>
       <c r="X68" s="54" t="str">
-        <f ca="1">IF(X67="","",IF(X66&gt;X67,"",ROUND(X67*(IF($P67="",$P66,$P67)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X67="","",IF(X66&gt;X67,"",ROUND(X67*(IF($P67="",$P66,$P67)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y68" s="54" t="str">
@@ -10111,8 +10186,14 @@
       </c>
       <c r="M69" s="20"/>
       <c r="N69" s="20"/>
-      <c r="O69" s="33"/>
-      <c r="P69" s="35"/>
+      <c r="O69" s="76" t="str">
+        <f>IF(P69="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P69" s="21" t="str">
+        <f>IF(A65="","",IF(VLOOKUP(A65,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A65,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="70" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="52" t="str">
@@ -10132,7 +10213,7 @@
         <f>IF(A70="","",VLOOKUP(A70,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F70" s="112" t="str">
+      <c r="F70" s="113" t="str">
         <f>IF(A70="","","Titulo:")</f>
         <v/>
       </c>
@@ -10149,7 +10230,7 @@
       <c r="N70" s="28"/>
       <c r="O70" s="28"/>
       <c r="P70" s="28"/>
-      <c r="Q70" s="112" t="str">
+      <c r="Q70" s="113" t="str">
         <f>IF(A70="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -10534,8 +10615,14 @@
       </c>
       <c r="M74" s="20"/>
       <c r="N74" s="20"/>
-      <c r="O74" s="33"/>
-      <c r="P74" s="35"/>
+      <c r="O74" s="76" t="str">
+        <f>IF(P74="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P74" s="21" t="str">
+        <f>IF(A70="","",IF(VLOOKUP(A70,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A70,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="75" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="52" t="str">
@@ -10555,7 +10642,7 @@
         <f>IF(A75="","",VLOOKUP(A75,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F75" s="112" t="str">
+      <c r="F75" s="113" t="str">
         <f>IF(A75="","","Titulo:")</f>
         <v/>
       </c>
@@ -10572,7 +10659,7 @@
       <c r="N75" s="28"/>
       <c r="O75" s="28"/>
       <c r="P75" s="28"/>
-      <c r="Q75" s="112" t="str">
+      <c r="Q75" s="113" t="str">
         <f>IF(A75="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -10957,8 +11044,14 @@
       </c>
       <c r="M79" s="20"/>
       <c r="N79" s="20"/>
-      <c r="O79" s="33"/>
-      <c r="P79" s="35"/>
+      <c r="O79" s="76" t="str">
+        <f>IF(P79="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P79" s="21" t="str">
+        <f>IF(A75="","",IF(VLOOKUP(A75,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A75,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="80" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="52" t="str">
@@ -10978,7 +11071,7 @@
         <f>IF(A80="","",VLOOKUP(A80,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F80" s="112" t="str">
+      <c r="F80" s="113" t="str">
         <f>IF(A80="","","Titulo:")</f>
         <v/>
       </c>
@@ -10995,7 +11088,7 @@
       <c r="N80" s="28"/>
       <c r="O80" s="28"/>
       <c r="P80" s="28"/>
-      <c r="Q80" s="112" t="str">
+      <c r="Q80" s="113" t="str">
         <f>IF(A80="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -11380,8 +11473,14 @@
       </c>
       <c r="M84" s="20"/>
       <c r="N84" s="20"/>
-      <c r="O84" s="33"/>
-      <c r="P84" s="35"/>
+      <c r="O84" s="76" t="str">
+        <f>IF(P84="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P84" s="21" t="str">
+        <f>IF(A80="","",IF(VLOOKUP(A80,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A80,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="85" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="52" t="str">
@@ -11401,7 +11500,7 @@
         <f>IF(A85="","",VLOOKUP(A85,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F85" s="112" t="str">
+      <c r="F85" s="113" t="str">
         <f>IF(A85="","","Titulo:")</f>
         <v/>
       </c>
@@ -11418,7 +11517,7 @@
       <c r="N85" s="28"/>
       <c r="O85" s="28"/>
       <c r="P85" s="28"/>
-      <c r="Q85" s="112" t="str">
+      <c r="Q85" s="113" t="str">
         <f>IF(A85="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -11803,8 +11902,14 @@
       </c>
       <c r="M89" s="20"/>
       <c r="N89" s="20"/>
-      <c r="O89" s="33"/>
-      <c r="P89" s="35"/>
+      <c r="O89" s="76" t="str">
+        <f>IF(P89="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P89" s="21" t="str">
+        <f>IF(A85="","",IF(VLOOKUP(A85,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A85,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="90" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="52" t="str">
@@ -11824,7 +11929,7 @@
         <f>IF(A90="","",VLOOKUP(A90,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F90" s="112" t="str">
+      <c r="F90" s="113" t="str">
         <f>IF(A90="","","Titulo:")</f>
         <v/>
       </c>
@@ -11841,7 +11946,7 @@
       <c r="N90" s="28"/>
       <c r="O90" s="28"/>
       <c r="P90" s="28"/>
-      <c r="Q90" s="112" t="str">
+      <c r="Q90" s="113" t="str">
         <f>IF(A90="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -12226,8 +12331,14 @@
       </c>
       <c r="M94" s="20"/>
       <c r="N94" s="20"/>
-      <c r="O94" s="33"/>
-      <c r="P94" s="35"/>
+      <c r="O94" s="76" t="str">
+        <f>IF(P94="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P94" s="21" t="str">
+        <f>IF(A90="","",IF(VLOOKUP(A90,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A90,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="95" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="52" t="str">
@@ -12247,7 +12358,7 @@
         <f>IF(A95="","",VLOOKUP(A95,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F95" s="112" t="str">
+      <c r="F95" s="113" t="str">
         <f>IF(A95="","","Titulo:")</f>
         <v/>
       </c>
@@ -12264,7 +12375,7 @@
       <c r="N95" s="28"/>
       <c r="O95" s="28"/>
       <c r="P95" s="28"/>
-      <c r="Q95" s="112" t="str">
+      <c r="Q95" s="113" t="str">
         <f>IF(A95="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -12649,8 +12760,14 @@
       </c>
       <c r="M99" s="20"/>
       <c r="N99" s="20"/>
-      <c r="O99" s="33"/>
-      <c r="P99" s="35"/>
+      <c r="O99" s="76" t="str">
+        <f>IF(P99="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P99" s="21" t="str">
+        <f>IF(A95="","",IF(VLOOKUP(A95,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A95,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="100" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="52" t="str">
@@ -12670,7 +12787,7 @@
         <f>IF(A100="","",VLOOKUP(A100,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F100" s="112" t="str">
+      <c r="F100" s="113" t="str">
         <f>IF(A100="","","Titulo:")</f>
         <v/>
       </c>
@@ -12687,7 +12804,7 @@
       <c r="N100" s="28"/>
       <c r="O100" s="28"/>
       <c r="P100" s="28"/>
-      <c r="Q100" s="112" t="str">
+      <c r="Q100" s="113" t="str">
         <f>IF(A100="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -13072,8 +13189,14 @@
       </c>
       <c r="M104" s="20"/>
       <c r="N104" s="20"/>
-      <c r="O104" s="33"/>
-      <c r="P104" s="35"/>
+      <c r="O104" s="76" t="str">
+        <f>IF(P104="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P104" s="21" t="str">
+        <f>IF(A100="","",IF(VLOOKUP(A100,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A100,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="105" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="52" t="str">
@@ -13093,7 +13216,7 @@
         <f>IF(A105="","",VLOOKUP(A105,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F105" s="112" t="str">
+      <c r="F105" s="113" t="str">
         <f>IF(A105="","","Titulo:")</f>
         <v/>
       </c>
@@ -13110,7 +13233,7 @@
       <c r="N105" s="28"/>
       <c r="O105" s="28"/>
       <c r="P105" s="28"/>
-      <c r="Q105" s="112" t="str">
+      <c r="Q105" s="113" t="str">
         <f>IF(A105="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -13495,8 +13618,14 @@
       </c>
       <c r="M109" s="20"/>
       <c r="N109" s="20"/>
-      <c r="O109" s="33"/>
-      <c r="P109" s="35"/>
+      <c r="O109" s="76" t="str">
+        <f>IF(P109="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P109" s="21" t="str">
+        <f>IF(A105="","",IF(VLOOKUP(A105,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A105,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="110" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="52" t="str">
@@ -13516,7 +13645,7 @@
         <f>IF(A110="","",VLOOKUP(A110,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F110" s="112" t="str">
+      <c r="F110" s="113" t="str">
         <f>IF(A110="","","Titulo:")</f>
         <v/>
       </c>
@@ -13533,7 +13662,7 @@
       <c r="N110" s="28"/>
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
-      <c r="Q110" s="112" t="str">
+      <c r="Q110" s="113" t="str">
         <f>IF(A110="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -13918,8 +14047,14 @@
       </c>
       <c r="M114" s="20"/>
       <c r="N114" s="20"/>
-      <c r="O114" s="33"/>
-      <c r="P114" s="35"/>
+      <c r="O114" s="76" t="str">
+        <f>IF(P114="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P114" s="21" t="str">
+        <f>IF(A110="","",IF(VLOOKUP(A110,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A110,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="115" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="52" t="str">
@@ -13939,7 +14074,7 @@
         <f>IF(A115="","",VLOOKUP(A115,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F115" s="112" t="str">
+      <c r="F115" s="113" t="str">
         <f>IF(A115="","","Titulo:")</f>
         <v/>
       </c>
@@ -13956,7 +14091,7 @@
       <c r="N115" s="28"/>
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
-      <c r="Q115" s="112" t="str">
+      <c r="Q115" s="113" t="str">
         <f>IF(A115="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -14341,8 +14476,14 @@
       </c>
       <c r="M119" s="20"/>
       <c r="N119" s="20"/>
-      <c r="O119" s="33"/>
-      <c r="P119" s="35"/>
+      <c r="O119" s="76" t="str">
+        <f>IF(P119="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P119" s="21" t="str">
+        <f>IF(A115="","",IF(VLOOKUP(A115,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A115,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="120" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="52" t="str">
@@ -14362,7 +14503,7 @@
         <f>IF(A120="","",VLOOKUP(A120,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F120" s="112" t="str">
+      <c r="F120" s="113" t="str">
         <f>IF(A120="","","Titulo:")</f>
         <v/>
       </c>
@@ -14379,7 +14520,7 @@
       <c r="N120" s="28"/>
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
-      <c r="Q120" s="112" t="str">
+      <c r="Q120" s="113" t="str">
         <f>IF(A120="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -14764,8 +14905,14 @@
       </c>
       <c r="M124" s="20"/>
       <c r="N124" s="20"/>
-      <c r="O124" s="33"/>
-      <c r="P124" s="35"/>
+      <c r="O124" s="76" t="str">
+        <f>IF(P124="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P124" s="21" t="str">
+        <f>IF(A120="","",IF(VLOOKUP(A120,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A120,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="125" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="52" t="str">
@@ -14785,7 +14932,7 @@
         <f>IF(A125="","",VLOOKUP(A125,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F125" s="112" t="str">
+      <c r="F125" s="113" t="str">
         <f>IF(A125="","","Titulo:")</f>
         <v/>
       </c>
@@ -14802,7 +14949,7 @@
       <c r="N125" s="28"/>
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
-      <c r="Q125" s="112" t="str">
+      <c r="Q125" s="113" t="str">
         <f>IF(A125="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -15187,8 +15334,14 @@
       </c>
       <c r="M129" s="20"/>
       <c r="N129" s="20"/>
-      <c r="O129" s="33"/>
-      <c r="P129" s="35"/>
+      <c r="O129" s="76" t="str">
+        <f>IF(P129="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P129" s="21" t="str">
+        <f>IF(A125="","",IF(VLOOKUP(A125,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A125,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="130" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="52" t="str">
@@ -15208,7 +15361,7 @@
         <f>IF(A130="","",VLOOKUP(A130,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F130" s="112" t="str">
+      <c r="F130" s="113" t="str">
         <f>IF(A130="","","Titulo:")</f>
         <v/>
       </c>
@@ -15225,7 +15378,7 @@
       <c r="N130" s="28"/>
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
-      <c r="Q130" s="112" t="str">
+      <c r="Q130" s="113" t="str">
         <f>IF(A130="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -15610,8 +15763,14 @@
       </c>
       <c r="M134" s="20"/>
       <c r="N134" s="20"/>
-      <c r="O134" s="33"/>
-      <c r="P134" s="35"/>
+      <c r="O134" s="76" t="str">
+        <f>IF(P134="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P134" s="21" t="str">
+        <f>IF(A130="","",IF(VLOOKUP(A130,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A130,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="135" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="52" t="str">
@@ -15631,7 +15790,7 @@
         <f>IF(A135="","",VLOOKUP(A135,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F135" s="112" t="str">
+      <c r="F135" s="113" t="str">
         <f>IF(A135="","","Titulo:")</f>
         <v/>
       </c>
@@ -15648,7 +15807,7 @@
       <c r="N135" s="28"/>
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
-      <c r="Q135" s="112" t="str">
+      <c r="Q135" s="113" t="str">
         <f>IF(A135="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -16033,8 +16192,14 @@
       </c>
       <c r="M139" s="20"/>
       <c r="N139" s="20"/>
-      <c r="O139" s="33"/>
-      <c r="P139" s="35"/>
+      <c r="O139" s="76" t="str">
+        <f>IF(P139="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P139" s="21" t="str">
+        <f>IF(A135="","",IF(VLOOKUP(A135,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A135,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="140" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="52" t="str">
@@ -16054,7 +16219,7 @@
         <f>IF(A140="","",VLOOKUP(A140,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F140" s="112" t="str">
+      <c r="F140" s="113" t="str">
         <f>IF(A140="","","Titulo:")</f>
         <v/>
       </c>
@@ -16071,7 +16236,7 @@
       <c r="N140" s="28"/>
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
-      <c r="Q140" s="112" t="str">
+      <c r="Q140" s="113" t="str">
         <f>IF(A140="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -16456,8 +16621,14 @@
       </c>
       <c r="M144" s="20"/>
       <c r="N144" s="20"/>
-      <c r="O144" s="33"/>
-      <c r="P144" s="35"/>
+      <c r="O144" s="76" t="str">
+        <f>IF(P144="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P144" s="21" t="str">
+        <f>IF(A140="","",IF(VLOOKUP(A140,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A140,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="145" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="52" t="str">
@@ -16477,7 +16648,7 @@
         <f>IF(A145="","",VLOOKUP(A145,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F145" s="112" t="str">
+      <c r="F145" s="113" t="str">
         <f>IF(A145="","","Titulo:")</f>
         <v/>
       </c>
@@ -16494,7 +16665,7 @@
       <c r="N145" s="28"/>
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
-      <c r="Q145" s="112" t="str">
+      <c r="Q145" s="113" t="str">
         <f>IF(A145="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -16879,8 +17050,14 @@
       </c>
       <c r="M149" s="20"/>
       <c r="N149" s="20"/>
-      <c r="O149" s="33"/>
-      <c r="P149" s="35"/>
+      <c r="O149" s="76" t="str">
+        <f>IF(P149="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P149" s="21" t="str">
+        <f>IF(A145="","",IF(VLOOKUP(A145,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A145,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
     <row r="150" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="52" t="str">
@@ -16900,7 +17077,7 @@
         <f>IF(A150="","",VLOOKUP(A150,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v/>
       </c>
-      <c r="F150" s="112" t="str">
+      <c r="F150" s="113" t="str">
         <f>IF(A150="","","Titulo:")</f>
         <v/>
       </c>
@@ -16917,7 +17094,7 @@
       <c r="N150" s="28"/>
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
-      <c r="Q150" s="112" t="str">
+      <c r="Q150" s="113" t="str">
         <f>IF(A150="","","Tipo da OS:")</f>
         <v/>
       </c>
@@ -17302,8 +17479,14 @@
       </c>
       <c r="M154" s="20"/>
       <c r="N154" s="20"/>
-      <c r="O154" s="33"/>
-      <c r="P154" s="35"/>
+      <c r="O154" s="76" t="str">
+        <f>IF(P154="","","Alteração")</f>
+        <v/>
+      </c>
+      <c r="P154" s="21" t="str">
+        <f>IF(A150="","",IF(VLOOKUP(A150,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A150,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -17352,10 +17535,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17364,104 +17547,132 @@
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>203</v>
       </c>
       <c r="B1" s="21">
-        <v>4757</v>
+        <v>4809</v>
       </c>
       <c r="E1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <f>IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("Abertura da OS",OSS[#Headers],0),FALSE))</f>
-        <v>42486</v>
+        <v>42591</v>
       </c>
       <c r="B2" t="s">
         <v>108</v>
       </c>
       <c r="E2" s="109" t="str">
         <f>TEXT(A2,"DD/MM/AA")&amp;" "&amp;B2&amp;IF(C2="",""," "&amp;TEXT(C2,"DD/MM/AA"))</f>
-        <v>26/04/16 Abertura</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>09/08/16 Abertura</v>
+      </c>
+      <c r="F2" s="67">
+        <f>IF(A3="","",ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))))-42))*30,0)+IF(VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
+        <v>158</v>
+      </c>
+      <c r="G2" s="109" t="str">
+        <f>IF(B1="","","Prazo previsto para execução em dias corridos")</f>
+        <v>Prazo previsto para execução em dias corridos</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <f>IF(A2="","",WORKDAY(A2,IF(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))&lt;150,5,10)))</f>
-        <v>42493</v>
+        <v>42598</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="20">
         <f>IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v>42493</v>
+        <v>42597</v>
       </c>
       <c r="E3" s="109" t="str">
         <f t="shared" ref="E3:E10" si="0">TEXT(A3,"DD/MM/AA")&amp;" "&amp;B3&amp;IF(C3="",""," "&amp;TEXT(C3,"DD/MM/AA"))</f>
-        <v>03/05/16 Inicio 03/05/16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16/08/16 Inicio 15/08/16</v>
+      </c>
+      <c r="F3" s="67">
+        <f>IF(A3="","",IF(IFERROR(VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE),0)=0,"",VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
+        <v>86</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(B1="","","Acréscimo no prazo previsto para execução em dias corridos")</f>
+        <v>Acréscimo no prazo previsto para execução em dias corridos</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>IF(A3="","",WORKDAY(A3,5))</f>
-        <v>42500</v>
+        <v>42605</v>
       </c>
       <c r="B4" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="20" t="str">
         <f>IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42500</v>
+        <v/>
       </c>
       <c r="E4" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>10/05/16 Entrega do Plano 10/05/16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23/08/16 Entrega do Plano</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <f>IF(A3="","",A3+ROUND(((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))))-42))*30*SLA_PrazoEntrega)+IF(VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
-        <v>42689</v>
+        <v>42727</v>
       </c>
       <c r="B5" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="20" t="str">
         <f>IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42639</v>
+        <v/>
       </c>
       <c r="E5" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>15/11/16 Entrega 26/09/16</v>
-      </c>
-      <c r="F5" s="20"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23/12/16 Entrega</v>
+      </c>
+      <c r="F5" s="112">
+        <f>IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE))</f>
+        <v>117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <f>IF(A5="","",WORKDAY(IF(C5="",A5,IF(C5&gt;A5,C5,A5)),IF(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))))&lt;150,5,10)))</f>
-        <v>42696</v>
+        <v>42734</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="20" t="str">
         <f>IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
-        <v>42600</v>
+        <v/>
       </c>
       <c r="E6" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>22/11/16 Recebimento 18/08/16</v>
-      </c>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30/12/16 Recebimento</v>
+      </c>
+      <c r="F6" s="112" t="str">
+        <f>IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))</f>
+        <v/>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <f>IF(A6="","",A6+ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))&gt;IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))),IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))&gt;IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))),IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)))))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42709</v>
+        <v>42748</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -17472,14 +17683,20 @@
       </c>
       <c r="E7" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>05/12/16 Aceite</v>
-      </c>
-      <c r="F7" s="20"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13/01/17 Aceite</v>
+      </c>
+      <c r="F7" s="112">
+        <f>IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <f>IF(A3="","",A3+ROUND((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))="",IF(B1="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[#Data],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))))-42))*30,0)+IF(VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[#Data],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)))</f>
-        <v>42715</v>
+        <f>IF(A3="","",A3+ROUND(((IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)))))/(19*LN(IF(IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))="",IF(B1="","",VLOOKUP(B1,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE)),IF(B1="","",IF(VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(B1,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)+IF(VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("PF Alterado",OSS[#Headers],0),FALSE))))))-42))*30)+IF(VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)="",0,VLOOKUP(B1,OSS[],MATCH("Acréscimo de Dias",OSS[#Headers],0),FALSE)),0))</f>
+        <v>42756</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
@@ -17490,13 +17707,13 @@
       </c>
       <c r="E8" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>11/12/16 Termino</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21/01/17 Termino</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <f>IF(A7="","",WORKDAY(A7,1))</f>
-        <v>42710</v>
+        <v>42751</v>
       </c>
       <c r="B9" t="s">
         <v>58</v>
@@ -17507,13 +17724,20 @@
       </c>
       <c r="E9" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>06/12/16 Garantia</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16/01/17 Garantia</v>
+      </c>
+      <c r="F9" s="112">
+        <f>IF(B1="","",ROUND((A8-A3)*SLA_ICP_EOS,1))</f>
+        <v>15.8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <f>IF(A9="","",A9+SLA_PrazoGarantia)</f>
-        <v>42890</v>
+        <v>42931</v>
       </c>
       <c r="B10" t="s">
         <v>107</v>
@@ -17524,7 +17748,14 @@
       </c>
       <c r="E10" s="109" t="str">
         <f t="shared" si="0"/>
-        <v>04/06/17 Fim da Garantia</v>
+        <v>15/07/17 Fim da Garantia</v>
+      </c>
+      <c r="F10" s="112">
+        <f>IF(B1="","",ROUND((A8-A3)*SLA_ICA_EOS,1))</f>
+        <v>39.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -17694,14 +17925,14 @@
       </c>
       <c r="F7" s="95">
         <f ca="1">Faturamento!J2</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G7" s="96">
         <v>699.62</v>
       </c>
       <c r="H7" s="97">
         <f ca="1">G7*F7</f>
-        <v>0</v>
+        <v>39178.720000000001</v>
       </c>
       <c r="J7" s="110"/>
       <c r="K7" s="110"/>
@@ -17824,7 +18055,7 @@
       <c r="G12" s="124"/>
       <c r="H12" s="100">
         <f ca="1">SUM(H5:H11)</f>
-        <v>0</v>
+        <v>39178.720000000001</v>
       </c>
       <c r="J12" s="110"/>
       <c r="K12" s="110"/>
@@ -17849,7 +18080,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:L8"/>
+      <selection sqref="A1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17883,7 +18114,7 @@
       <c r="K1" s="51"/>
       <c r="L1" s="80" t="str">
         <f ca="1">IF(ControleOSsMês!$B$1="Todas","Ref. Todas as OS","Ref. "&amp;UPPER(TEXT(ControleOSsMês!$F$1,"MMM/AAAA")))</f>
-        <v>Ref. OUT/2016</v>
+        <v>Ref. NOV/2016</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -17898,12 +18129,12 @@
       </c>
       <c r="J2" s="78">
         <f ca="1">SUM(Faturamento[PF a Faturar])</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K2" s="78"/>
       <c r="L2" s="73">
         <f ca="1">SUM(Faturamento[Valor a Faturar])</f>
-        <v>0</v>
+        <v>39178.720000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -17945,53 +18176,53 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="str">
+      <c r="A4" s="71">
         <f ca="1">IF(B4="","",ROW()-ROW($A$3))</f>
-        <v/>
-      </c>
-      <c r="B4" s="68" t="str">
+        <v>1</v>
+      </c>
+      <c r="B4" s="68">
         <f ca="1">IFERROR(VLOOKUP(ROW()-ROW($A$3),FatCTL[],2,FALSE),"")</f>
-        <v/>
+        <v>4797</v>
       </c>
       <c r="C4" s="69" t="str">
         <f ca="1">IF(B4="","",VLOOKUP(B4,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>PF Java</v>
       </c>
       <c r="D4" s="69" t="str">
         <f ca="1">IF(B4="","",VLOOKUP(B4,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v/>
-      </c>
-      <c r="E4" s="85" t="str">
+        <v>Recebida</v>
+      </c>
+      <c r="E4" s="85">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="",VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE),VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
-        <v/>
-      </c>
-      <c r="F4" s="84" t="str">
+        <v>53</v>
+      </c>
+      <c r="F4" s="84">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+1,5)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+1,5)))</f>
-        <v/>
-      </c>
-      <c r="G4" s="77" t="str">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(Faturamento[[#This Row],[Número OS]],Mensal!$A$5:$A$154,0)+1,4)))</f>
-        <v/>
-      </c>
-      <c r="H4" s="77" t="str">
+        <v>56</v>
+      </c>
+      <c r="H4" s="77">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+3,4)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+3,4)))</f>
-        <v/>
-      </c>
-      <c r="I4" s="77" t="str">
+        <v>0</v>
+      </c>
+      <c r="I4" s="77">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",IF(VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)="",0,VLOOKUP(Faturamento[[#This Row],[Número OS]],OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE)))</f>
-        <v/>
-      </c>
-      <c r="J4" s="77" t="str">
+        <v>0</v>
+      </c>
+      <c r="J4" s="77">
         <f ca="1">IF(B4="","",IF(INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+4,3)="",0,INDEX(Mensal!$A$5:$AG$154,MATCH(B4,Mensal!$A$5:$A$154,0)+4,3)))</f>
-        <v/>
-      </c>
-      <c r="K4" s="72" t="str">
+        <v>56</v>
+      </c>
+      <c r="K4" s="72">
         <f ca="1">IF(Faturamento[[#This Row],[Número OS]]="","",VLOOKUP(Faturamento[[#This Row],[Tipo da OS]],TipoOS[],2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="L4" s="72" t="str">
+        <v>699.62</v>
+      </c>
+      <c r="L4" s="72">
         <f ca="1">IF(B4="","",J4*Faturamento[[#This Row],[Valor Unitario]])</f>
-        <v/>
+        <v>39178.720000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -19206,7 +19437,7 @@
       </c>
       <c r="C1" s="58" t="str">
         <f ca="1">YEAR(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1)&amp;TEXT(MONTH(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1),"00")</f>
-        <v>201609</v>
+        <v>201610</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" t="s">
@@ -19214,11 +19445,11 @@
       </c>
       <c r="F1" s="20">
         <f ca="1">IF($G$1="",TODAY(),$G$1)</f>
-        <v>42674</v>
+        <v>42689</v>
       </c>
       <c r="G1" s="50">
         <f>IF(Mensal!B1="","",Mensal!B1)</f>
-        <v>42674</v>
+        <v>42689</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -19327,7 +19558,7 @@
       </c>
       <c r="F5" s="50">
         <f>IF(C5="","",VLOOKUP(C5,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
+        <v>42679</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" si="1"/>
@@ -19358,7 +19589,7 @@
       </c>
       <c r="F6" s="50">
         <f>IF(C6="","",VLOOKUP(C6,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
+        <v>42679</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
@@ -19389,7 +19620,7 @@
       </c>
       <c r="F7" s="50">
         <f>IF(C7="","",VLOOKUP(C7,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42675</v>
+        <v>42682</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
@@ -19575,7 +19806,7 @@
       </c>
       <c r="F13" s="50">
         <f>IF(C13="","",VLOOKUP(C13,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42677</v>
+        <v>42684</v>
       </c>
       <c r="G13" s="21">
         <f t="shared" si="1"/>
@@ -19605,7 +19836,7 @@
       </c>
       <c r="F14" s="50">
         <f>IF(C14="","",VLOOKUP(C14,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42677</v>
+        <v>42684</v>
       </c>
       <c r="G14" s="21">
         <f t="shared" si="1"/>
@@ -19635,7 +19866,7 @@
       </c>
       <c r="F15" s="50">
         <f>IF(C15="","",VLOOKUP(C15,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42688</v>
+        <v>42695</v>
       </c>
       <c r="G15" s="21">
         <f t="shared" si="1"/>

</xml_diff>